<commit_message>
Update Input List.xlsx with new data
</commit_message>
<xml_diff>
--- a/Input List/FullBand/Input List.xlsx
+++ b/Input List/FullBand/Input List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\TechnicalDocumentation\Input List\FullBand\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416A4561-2467-4D2C-B1A6-BBA56D6326CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7257A137-28E8-4F9A-833C-6575543BF8C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{976BA9A3-41FE-45E5-BC0B-B40312D9AF21}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="159">
   <si>
     <t>Input</t>
   </si>
@@ -425,9 +425,6 @@
     <t>Paul Acoustic</t>
   </si>
   <si>
-    <t>Guest 1 Vocals</t>
-  </si>
-  <si>
     <t>Billy
 IEM Left</t>
   </si>
@@ -570,6 +567,15 @@
   </si>
   <si>
     <t>Mike Acoustic</t>
+  </si>
+  <si>
+    <t>Mike's IEM</t>
+  </si>
+  <si>
+    <t>???</t>
+  </si>
+  <si>
+    <t>Guest Vocals</t>
   </si>
 </sst>
 </file>
@@ -1123,16 +1129,61 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -1167,24 +1218,72 @@
     <xf numFmtId="0" fontId="19" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1227,103 +1326,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1422,8 +1428,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F06299C-206A-4E5B-812B-2628B9127415}" name="Table1" displayName="Table1" ref="K19:M24" totalsRowShown="0">
-  <autoFilter ref="K19:M24" xr:uid="{1F06299C-206A-4E5B-812B-2628B9127415}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F06299C-206A-4E5B-812B-2628B9127415}" name="Table1" displayName="Table1" ref="K19:M25" totalsRowShown="0">
+  <autoFilter ref="K19:M25" xr:uid="{1F06299C-206A-4E5B-812B-2628B9127415}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{DBD1845E-C8E6-4D25-AB4B-500331BD2BF7}" name="Device"/>
     <tableColumn id="2" xr3:uid="{25C87226-CD3A-436C-AE3E-D8E60BFFEA83}" name="Model"/>
@@ -1732,8 +1738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A11D25-D77D-4358-9E34-E04B11CA4C7B}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1750,29 +1756,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="e" vm="1">
+      <c r="A1" s="59" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="46" t="s">
+      <c r="B1" s="59"/>
+      <c r="C1" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
       <c r="H1" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="62"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="62"/>
       <c r="H2" s="9" t="str">
         <f ca="1">"Date Updated: "&amp;TEXT(TODAY(),"yyyy.mm.dd")</f>
         <v>Date Updated: 2026.02.03</v>
@@ -1786,13 +1792,13 @@
         <v>59</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D3" s="16" t="s">
         <v>63</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F3" s="16" t="s">
         <v>15</v>
@@ -1805,10 +1811,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="66" t="s">
         <v>22</v>
       </c>
       <c r="C4" s="17">
@@ -1831,8 +1837,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49"/>
-      <c r="B5" s="52"/>
+      <c r="A5" s="64"/>
+      <c r="B5" s="67"/>
       <c r="C5" s="19">
         <v>2</v>
       </c>
@@ -1853,8 +1859,8 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49"/>
-      <c r="B6" s="52"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="67"/>
       <c r="C6" s="17">
         <v>3</v>
       </c>
@@ -1873,8 +1879,8 @@
       <c r="H6" s="18"/>
     </row>
     <row r="7" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49"/>
-      <c r="B7" s="52"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="67"/>
       <c r="C7" s="19">
         <v>4</v>
       </c>
@@ -1895,8 +1901,8 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49"/>
-      <c r="B8" s="52"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="67"/>
       <c r="C8" s="17">
         <v>5</v>
       </c>
@@ -1917,8 +1923,8 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49"/>
-      <c r="B9" s="52"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="67"/>
       <c r="C9" s="19">
         <v>6</v>
       </c>
@@ -1939,8 +1945,8 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49"/>
-      <c r="B10" s="52"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="67"/>
       <c r="C10" s="17">
         <v>7</v>
       </c>
@@ -1961,8 +1967,8 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49"/>
-      <c r="B11" s="52"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="67"/>
       <c r="C11" s="19">
         <v>8</v>
       </c>
@@ -1983,8 +1989,8 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49"/>
-      <c r="B12" s="52"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="67"/>
       <c r="C12" s="17">
         <v>9</v>
       </c>
@@ -2005,8 +2011,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50"/>
-      <c r="B13" s="53"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="68"/>
       <c r="C13" s="19">
         <v>10</v>
       </c>
@@ -2033,12 +2039,12 @@
         <v>11</v>
       </c>
       <c r="D14" s="22"/>
-      <c r="E14" s="40" t="s">
+      <c r="E14" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
+      <c r="F14" s="48"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="48"/>
     </row>
     <row r="15" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
@@ -2047,12 +2053,12 @@
         <v>12</v>
       </c>
       <c r="D15" s="22"/>
-      <c r="E15" s="40" t="s">
+      <c r="E15" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
     </row>
     <row r="16" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
@@ -2061,19 +2067,19 @@
         <v>13</v>
       </c>
       <c r="D16" s="22"/>
-      <c r="E16" s="40" t="s">
+      <c r="E16" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
+      <c r="F16" s="48"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="48"/>
     </row>
     <row r="17" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="102" t="s">
+      <c r="A17" s="55" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="103" t="s">
-        <v>141</v>
+      <c r="B17" s="56" t="s">
+        <v>140</v>
       </c>
       <c r="C17" s="23">
         <v>14</v>
@@ -2095,8 +2101,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="102"/>
-      <c r="B18" s="103"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
       <c r="C18" s="25">
         <v>15</v>
       </c>
@@ -2121,19 +2127,19 @@
         <v>16</v>
       </c>
       <c r="D19" s="22"/>
-      <c r="E19" s="40" t="s">
+      <c r="E19" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
     </row>
     <row r="20" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="43" t="s">
+      <c r="A20" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="43" t="s">
-        <v>142</v>
+      <c r="B20" s="69" t="s">
+        <v>141</v>
       </c>
       <c r="C20" s="28">
         <v>17</v>
@@ -2155,8 +2161,8 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="43"/>
-      <c r="B21" s="43"/>
+      <c r="A21" s="69"/>
+      <c r="B21" s="69"/>
       <c r="C21" s="30">
         <v>18</v>
       </c>
@@ -2175,31 +2181,31 @@
       <c r="H21" s="31"/>
     </row>
     <row r="22" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="104"/>
-      <c r="B22" s="104"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="21">
         <v>19</v>
       </c>
       <c r="D22" s="22"/>
-      <c r="E22" s="40" t="s">
+      <c r="E22" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="40"/>
-      <c r="G22" s="40"/>
-      <c r="H22" s="40"/>
+      <c r="F22" s="48"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="48"/>
     </row>
     <row r="23" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="105" t="s">
+      <c r="A23" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="B23" s="105" t="s">
-        <v>143</v>
+      <c r="B23" s="57" t="s">
+        <v>142</v>
       </c>
       <c r="C23" s="32">
         <v>20</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E23" s="33" t="s">
         <v>1</v>
@@ -2215,8 +2221,8 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="105"/>
-      <c r="B24" s="105"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="57"/>
       <c r="C24" s="34">
         <v>21</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>80</v>
       </c>
       <c r="E24" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F24" s="35" t="s">
         <v>31</v>
@@ -2235,8 +2241,8 @@
       <c r="H24" s="35"/>
     </row>
     <row r="25" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="105"/>
-      <c r="B25" s="105"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="57"/>
       <c r="C25" s="32">
         <v>22</v>
       </c>
@@ -2244,7 +2250,7 @@
         <v>104</v>
       </c>
       <c r="E25" s="33" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F25" s="33" t="s">
         <v>31</v>
@@ -2255,13 +2261,13 @@
       <c r="H25" s="33"/>
     </row>
     <row r="26" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="105"/>
-      <c r="B26" s="105"/>
+      <c r="A26" s="57"/>
+      <c r="B26" s="57"/>
       <c r="C26" s="34">
         <v>23</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E26" s="35" t="s">
         <v>114</v>
@@ -2275,91 +2281,91 @@
       <c r="H26" s="35"/>
     </row>
     <row r="27" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="106" t="s">
+      <c r="A27" s="58" t="s">
+        <v>151</v>
+      </c>
+      <c r="B27" s="58" t="s">
         <v>152</v>
       </c>
-      <c r="B27" s="106" t="s">
+      <c r="C27" s="43">
+        <v>24</v>
+      </c>
+      <c r="D27" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="C27" s="98">
-        <v>24</v>
-      </c>
-      <c r="D27" s="99" t="s">
+      <c r="F27" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="H27" s="44" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="58"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="45">
+        <v>25</v>
+      </c>
+      <c r="D28" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="E27" s="99" t="s">
+      <c r="E28" s="46" t="s">
         <v>154</v>
       </c>
-      <c r="F27" s="99" t="s">
+      <c r="F28" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="G27" s="99" t="s">
-        <v>65</v>
-      </c>
-      <c r="H27" s="99" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="106"/>
-      <c r="B28" s="106"/>
-      <c r="C28" s="100">
-        <v>25</v>
-      </c>
-      <c r="D28" s="101" t="s">
+      <c r="G28" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="H28" s="46"/>
+    </row>
+    <row r="29" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="58"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="43">
+        <v>26</v>
+      </c>
+      <c r="D29" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E28" s="101" t="s">
+      <c r="E29" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="F28" s="101" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28" s="101" t="s">
-        <v>66</v>
-      </c>
-      <c r="H28" s="101"/>
-    </row>
-    <row r="29" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="106"/>
-      <c r="B29" s="106"/>
-      <c r="C29" s="98">
-        <v>26</v>
-      </c>
-      <c r="D29" s="99" t="s">
+      <c r="F29" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="G29" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="E29" s="99" t="s">
-        <v>156</v>
-      </c>
-      <c r="F29" s="99" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="H29" s="99"/>
+      <c r="H29" s="44"/>
     </row>
     <row r="30" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="104"/>
-      <c r="B30" s="104"/>
+      <c r="A30" s="47"/>
+      <c r="B30" s="47"/>
       <c r="C30" s="21">
         <v>27</v>
       </c>
       <c r="D30" s="22"/>
-      <c r="E30" s="40" t="s">
+      <c r="E30" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F30" s="40"/>
-      <c r="G30" s="40"/>
-      <c r="H30" s="40"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="48"/>
     </row>
     <row r="31" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="95" t="s">
+      <c r="A31" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="B31" s="54" t="s">
-        <v>144</v>
+      <c r="B31" s="52" t="s">
+        <v>143</v>
       </c>
       <c r="C31" s="36">
         <v>28</v>
@@ -2379,8 +2385,8 @@
       <c r="H31" s="36"/>
     </row>
     <row r="32" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="96"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="50"/>
+      <c r="B32" s="53"/>
       <c r="C32" s="37">
         <v>29</v>
       </c>
@@ -2401,8 +2407,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="96"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="50"/>
+      <c r="B33" s="53"/>
       <c r="C33" s="36">
         <v>30</v>
       </c>
@@ -2421,8 +2427,8 @@
       <c r="H33" s="36"/>
     </row>
     <row r="34" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="97"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="51"/>
+      <c r="B34" s="54"/>
       <c r="C34" s="37">
         <v>31</v>
       </c>
@@ -2441,31 +2447,31 @@
       <c r="H34" s="37"/>
     </row>
     <row r="35" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="92" t="s">
+      <c r="A35" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="B35" s="40" t="s">
         <v>135</v>
       </c>
-      <c r="B35" s="92" t="s">
-        <v>136</v>
-      </c>
-      <c r="C35" s="93">
+      <c r="C35" s="41">
         <v>32</v>
       </c>
-      <c r="D35" s="94"/>
-      <c r="E35" s="94" t="s">
-        <v>115</v>
-      </c>
-      <c r="F35" s="94" t="s">
+      <c r="D35" s="42"/>
+      <c r="E35" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="G35" s="94" t="s">
+      <c r="G35" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="H35" s="94" t="s">
+      <c r="H35" s="42" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="41" t="s">
+      <c r="A36" s="70" t="s">
         <v>49</v>
       </c>
       <c r="B36" s="11" t="s">
@@ -2491,7 +2497,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="42"/>
+      <c r="A37" s="71"/>
       <c r="B37" s="14"/>
       <c r="C37" s="21">
         <v>34</v>
@@ -2505,7 +2511,7 @@
       <c r="H37" s="13"/>
     </row>
     <row r="38" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="42"/>
+      <c r="A38" s="71"/>
       <c r="B38" s="14"/>
       <c r="C38" s="21">
         <v>35</v>
@@ -2519,7 +2525,7 @@
       <c r="H38" s="13"/>
     </row>
     <row r="39" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
+      <c r="A39" s="71"/>
       <c r="B39" s="14"/>
       <c r="C39" s="21">
         <v>36</v>
@@ -2533,21 +2539,21 @@
       <c r="H39" s="13"/>
     </row>
     <row r="40" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="42"/>
+      <c r="A40" s="71"/>
       <c r="B40" s="14"/>
       <c r="C40" s="21">
         <v>37</v>
       </c>
       <c r="D40" s="27"/>
-      <c r="E40" s="40" t="s">
+      <c r="E40" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F40" s="40"/>
-      <c r="G40" s="40"/>
-      <c r="H40" s="40"/>
+      <c r="F40" s="48"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="48"/>
     </row>
     <row r="41" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="42"/>
+      <c r="A41" s="71"/>
       <c r="B41" s="11" t="s">
         <v>29</v>
       </c>
@@ -2569,21 +2575,21 @@
       <c r="H41" s="39"/>
     </row>
     <row r="42" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="42"/>
+      <c r="A42" s="71"/>
       <c r="B42" s="14"/>
       <c r="C42" s="21">
         <v>39</v>
       </c>
       <c r="D42" s="27"/>
-      <c r="E42" s="40" t="s">
+      <c r="E42" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="F42" s="40"/>
-      <c r="G42" s="40"/>
-      <c r="H42" s="40"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="48"/>
     </row>
     <row r="43" spans="1:8" ht="11.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="42"/>
+      <c r="A43" s="71"/>
       <c r="B43" s="11" t="s">
         <v>111</v>
       </c>
@@ -2606,6 +2612,16 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E40:H40"/>
+    <mergeCell ref="A36:A43"/>
+    <mergeCell ref="E42:H42"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:G2"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="E14:H14"/>
+    <mergeCell ref="E16:H16"/>
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="B4:B13"/>
     <mergeCell ref="E30:H30"/>
     <mergeCell ref="A31:A34"/>
     <mergeCell ref="B31:B34"/>
@@ -2615,20 +2631,10 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:B29"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:G2"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="E14:H14"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="B4:B13"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="E19:H19"/>
     <mergeCell ref="E22:H22"/>
-    <mergeCell ref="E40:H40"/>
-    <mergeCell ref="A36:A43"/>
-    <mergeCell ref="E42:H42"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2641,7 +2647,7 @@
   <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView topLeftCell="A16" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2655,86 +2661,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="e" vm="1">
+      <c r="A1" s="59" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="46" t="str">
+      <c r="B1" s="59"/>
+      <c r="C1" s="61" t="str">
         <f>Channels!C1</f>
         <v>Full Band Setup</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="74" t="str">
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="87" t="str">
         <f>Channels!H1</f>
         <v>🌐 theperfectstrangers.band</v>
       </c>
-      <c r="L1" s="74"/>
-      <c r="M1" s="74"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
       <c r="P1" s="7"/>
     </row>
     <row r="2" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="78" t="str">
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="89" t="str">
         <f ca="1">Channels!H2</f>
         <v>Date Updated: 2026.02.03</v>
       </c>
-      <c r="L2" s="78"/>
-      <c r="M2" s="78"/>
+      <c r="L2" s="89"/>
+      <c r="M2" s="89"/>
     </row>
     <row r="3" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="76" t="s">
+      <c r="A3" s="75" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="76"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
+      <c r="B3" s="75"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
       <c r="I3" s="2"/>
-      <c r="K3" s="61" t="s">
+      <c r="K3" s="92" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="61"/>
-      <c r="M3" s="61"/>
+      <c r="L3" s="92"/>
+      <c r="M3" s="92"/>
     </row>
     <row r="4" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
-      <c r="H4" s="76"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
       <c r="I4" s="2"/>
-      <c r="K4" s="72">
+      <c r="K4" s="103">
         <v>1</v>
       </c>
-      <c r="L4" s="62" t="s">
+      <c r="L4" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="M4" s="63"/>
+      <c r="M4" s="94"/>
     </row>
     <row r="5" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -2762,9 +2768,9 @@
         <v>8</v>
       </c>
       <c r="I5" s="2"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="65"/>
+      <c r="K5" s="104"/>
+      <c r="L5" s="95"/>
+      <c r="M5" s="96"/>
     </row>
     <row r="6" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
@@ -2788,17 +2794,17 @@
       <c r="G6" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="84" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="2"/>
-      <c r="K6" s="70">
+      <c r="K6" s="101">
         <v>2</v>
       </c>
-      <c r="L6" s="66" t="s">
-        <v>131</v>
-      </c>
-      <c r="M6" s="67"/>
+      <c r="L6" s="97" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6" s="98"/>
     </row>
     <row r="7" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="77"/>
@@ -2808,11 +2814,11 @@
       <c r="E7" s="77"/>
       <c r="F7" s="77"/>
       <c r="G7" s="77"/>
-      <c r="H7" s="82"/>
+      <c r="H7" s="85"/>
       <c r="I7" s="2"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="68"/>
-      <c r="M7" s="69"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="100"/>
     </row>
     <row r="8" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -2824,13 +2830,13 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="2"/>
-      <c r="K8" s="72">
+      <c r="K8" s="103">
         <v>3</v>
       </c>
-      <c r="L8" s="62" t="s">
+      <c r="L8" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="M8" s="63"/>
+      <c r="M8" s="94"/>
     </row>
     <row r="9" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -2858,55 +2864,55 @@
         <v>16</v>
       </c>
       <c r="I9" s="2"/>
-      <c r="K9" s="73"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="65"/>
+      <c r="K9" s="104"/>
+      <c r="L9" s="95"/>
+      <c r="M9" s="96"/>
     </row>
     <row r="10" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="81" t="s">
+      <c r="A10" s="84" t="s">
         <v>43</v>
       </c>
       <c r="B10" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
       <c r="I10" s="2"/>
-      <c r="K10" s="70">
+      <c r="K10" s="101">
         <v>4</v>
       </c>
-      <c r="L10" s="66" t="s">
-        <v>132</v>
-      </c>
-      <c r="M10" s="67"/>
+      <c r="L10" s="97" t="s">
+        <v>131</v>
+      </c>
+      <c r="M10" s="98"/>
     </row>
     <row r="11" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
+      <c r="A11" s="85"/>
       <c r="B11" s="77"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
       <c r="I11" s="2"/>
-      <c r="K11" s="71"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="69"/>
+      <c r="K11" s="102"/>
+      <c r="L11" s="99"/>
+      <c r="M11" s="100"/>
     </row>
     <row r="12" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="2"/>
-      <c r="K12" s="72">
+      <c r="K12" s="103">
         <v>5</v>
       </c>
-      <c r="L12" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="M12" s="63"/>
+      <c r="L12" s="93" t="s">
+        <v>132</v>
+      </c>
+      <c r="M12" s="94"/>
     </row>
     <row r="13" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
@@ -2934,64 +2940,64 @@
         <v>24</v>
       </c>
       <c r="I13" s="2"/>
-      <c r="K13" s="73"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="65"/>
+      <c r="K13" s="104"/>
+      <c r="L13" s="95"/>
+      <c r="M13" s="96"/>
     </row>
     <row r="14" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="90" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="90" t="s">
         <v>123</v>
       </c>
-      <c r="B14" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="58" t="s">
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="90" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="58" t="s">
+      <c r="F14" s="90" t="s">
         <v>58</v>
       </c>
-      <c r="G14" s="57"/>
-      <c r="H14" s="58" t="s">
+      <c r="G14" s="86"/>
+      <c r="H14" s="90" t="s">
         <v>111</v>
       </c>
       <c r="I14" s="2"/>
-      <c r="K14" s="70">
+      <c r="K14" s="101">
         <v>6</v>
       </c>
-      <c r="L14" s="66"/>
-      <c r="M14" s="67"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="98"/>
     </row>
     <row r="15" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="58"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="57"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="G15" s="57"/>
-      <c r="H15" s="58"/>
+      <c r="A15" s="90"/>
+      <c r="B15" s="90"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="90"/>
       <c r="I15" s="2"/>
-      <c r="K15" s="71"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="69"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="100"/>
     </row>
     <row r="16" spans="1:16" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="2"/>
     </row>
     <row r="17" spans="1:13" ht="14.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="75"/>
       <c r="I17" s="6"/>
     </row>
     <row r="18" spans="1:13" ht="14.1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -3020,36 +3026,36 @@
         <v>8</v>
       </c>
       <c r="I18" s="2"/>
-      <c r="K18" s="60" t="s">
+      <c r="K18" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="L18" s="60"/>
-      <c r="M18" s="60"/>
+      <c r="L18" s="91"/>
+      <c r="M18" s="91"/>
     </row>
     <row r="19" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="79" t="s">
+      <c r="A19" s="72" t="s">
+        <v>115</v>
+      </c>
+      <c r="B19" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="79" t="s">
+      <c r="C19" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="E19" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="80" t="s">
-        <v>128</v>
-      </c>
-      <c r="D19" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="E19" s="59" t="s">
+      <c r="F19" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="F19" s="59" t="s">
-        <v>119</v>
-      </c>
-      <c r="G19" s="75" t="s">
+      <c r="G19" s="88" t="s">
+        <v>124</v>
+      </c>
+      <c r="H19" s="88" t="s">
         <v>125</v>
-      </c>
-      <c r="H19" s="75" t="s">
-        <v>126</v>
       </c>
       <c r="I19" s="2"/>
       <c r="K19" t="s">
@@ -3063,14 +3069,14 @@
       </c>
     </row>
     <row r="20" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
-      <c r="B20" s="79"/>
-      <c r="C20" s="80"/>
-      <c r="D20" s="80"/>
-      <c r="E20" s="59"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
+      <c r="A20" s="72"/>
+      <c r="B20" s="72"/>
+      <c r="C20" s="73"/>
+      <c r="D20" s="73"/>
+      <c r="E20" s="74"/>
+      <c r="F20" s="74"/>
+      <c r="G20" s="88"/>
+      <c r="H20" s="88"/>
       <c r="I20" s="2"/>
       <c r="K20" t="s">
         <v>95</v>
@@ -3115,16 +3121,16 @@
       </c>
     </row>
     <row r="23" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="75" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="76"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
-      <c r="F23" s="76"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
+      <c r="B23" s="75"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="75"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
       <c r="I23" s="2"/>
       <c r="K23" t="s">
         <v>98</v>
@@ -3137,16 +3143,16 @@
       </c>
     </row>
     <row r="24" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="76"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="75"/>
       <c r="I24" s="2"/>
       <c r="K24" t="s">
         <v>110</v>
@@ -3184,43 +3190,52 @@
         <v>8</v>
       </c>
       <c r="I25" s="2"/>
+      <c r="K25" t="s">
+        <v>156</v>
+      </c>
+      <c r="L25" t="s">
+        <v>157</v>
+      </c>
+      <c r="M25" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="26" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="83" t="s">
+      <c r="A26" s="105" t="s">
         <v>105</v>
       </c>
-      <c r="B26" s="79" t="s">
+      <c r="B26" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="C26" s="80" t="s">
+      <c r="C26" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="D26" s="80" t="s">
+      <c r="D26" s="73" t="s">
         <v>50</v>
       </c>
-      <c r="E26" s="59" t="s">
+      <c r="E26" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F26" s="59" t="s">
-        <v>140</v>
-      </c>
-      <c r="G26" s="59" t="s">
-        <v>146</v>
-      </c>
-      <c r="H26" s="59" t="s">
+      <c r="F26" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>145</v>
+      </c>
+      <c r="H26" s="74" t="s">
         <v>114</v>
       </c>
       <c r="I26" s="2"/>
     </row>
     <row r="27" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="84"/>
-      <c r="B27" s="79"/>
-      <c r="C27" s="80"/>
-      <c r="D27" s="80"/>
-      <c r="E27" s="59"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
+      <c r="A27" s="106"/>
+      <c r="B27" s="72"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
       <c r="I27" s="2"/>
     </row>
     <row r="28" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3262,57 +3277,57 @@
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="91" t="s">
+      <c r="A30" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="B30" s="82" t="s">
         <v>147</v>
       </c>
-      <c r="B30" s="89" t="s">
+      <c r="C30" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="C30" s="89" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="85" t="s">
+      <c r="D30" s="79" t="s">
         <v>4</v>
       </c>
-      <c r="E30" s="85" t="s">
+      <c r="E30" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="85" t="s">
+      <c r="F30" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="85" t="s">
+      <c r="G30" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="H30" s="87" t="s">
-        <v>115</v>
+      <c r="H30" s="81" t="s">
+        <v>158</v>
       </c>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="91"/>
-      <c r="B31" s="90"/>
-      <c r="C31" s="90"/>
-      <c r="D31" s="86"/>
-      <c r="E31" s="86"/>
-      <c r="F31" s="86"/>
-      <c r="G31" s="86"/>
-      <c r="H31" s="87"/>
+      <c r="A31" s="78"/>
+      <c r="B31" s="83"/>
+      <c r="C31" s="83"/>
+      <c r="D31" s="80"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="80"/>
+      <c r="G31" s="80"/>
+      <c r="H31" s="81"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:13" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="76"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="76"/>
-      <c r="E33" s="76"/>
-      <c r="F33" s="76"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
@@ -3344,78 +3359,74 @@
     </row>
     <row r="35" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="77" t="s">
+        <v>119</v>
+      </c>
+      <c r="B35" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="B35" s="77" t="s">
+      <c r="C35" s="78" t="s">
+        <v>149</v>
+      </c>
+      <c r="D35" s="78" t="s">
+        <v>150</v>
+      </c>
+      <c r="E35" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C35" s="91" t="s">
-        <v>150</v>
-      </c>
-      <c r="D35" s="91" t="s">
-        <v>151</v>
-      </c>
-      <c r="E35" s="88" t="s">
-        <v>122</v>
-      </c>
-      <c r="F35" s="88" t="s">
+      <c r="F35" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="76" t="s">
+        <v>107</v>
+      </c>
+      <c r="H35" s="76" t="s">
         <v>129</v>
-      </c>
-      <c r="G35" s="88" t="s">
-        <v>107</v>
-      </c>
-      <c r="H35" s="88" t="s">
-        <v>130</v>
       </c>
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="77"/>
       <c r="B36" s="77"/>
-      <c r="C36" s="91"/>
-      <c r="D36" s="91"/>
-      <c r="E36" s="88"/>
-      <c r="F36" s="88"/>
-      <c r="G36" s="88"/>
-      <c r="H36" s="88"/>
+      <c r="C36" s="78"/>
+      <c r="D36" s="78"/>
+      <c r="E36" s="76"/>
+      <c r="F36" s="76"/>
+      <c r="G36" s="76"/>
+      <c r="H36" s="76"/>
       <c r="I36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="80">
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A33:H33"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="H35:H36"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="F35:F36"/>
-    <mergeCell ref="F30:F31"/>
-    <mergeCell ref="G30:G31"/>
-    <mergeCell ref="H30:H31"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="D30:D31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:J2"/>
-    <mergeCell ref="G6:G7"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="K18:M18"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="L4:M5"/>
+    <mergeCell ref="L6:M7"/>
+    <mergeCell ref="L8:M9"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="K4:K5"/>
+    <mergeCell ref="L10:M11"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:M15"/>
     <mergeCell ref="K1:M1"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="D10:D11"/>
@@ -3432,36 +3443,40 @@
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="A14:A15"/>
-    <mergeCell ref="K18:M18"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="L4:M5"/>
-    <mergeCell ref="L6:M7"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="K4:K5"/>
-    <mergeCell ref="L10:M11"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:M15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A23:H23"/>
-    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:J2"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="D30:D31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="F30:F31"/>
+    <mergeCell ref="G30:G31"/>
+    <mergeCell ref="H30:H31"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="A33:H33"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="F35:F36"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>